<commit_message>
Fixed problem in intervention recommendations file where I had some formatting waaaaay down in the file that made it huge.
</commit_message>
<xml_diff>
--- a/design/recommendations_intervention_filledin.xlsx
+++ b/design/recommendations_intervention_filledin.xlsx
@@ -665,100 +665,7 @@
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF80FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF80FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF80FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1179,13 +1086,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DF1048545"/>
+  <dimension ref="A1:DF15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.109375" defaultRowHeight="18" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.109375" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.5546875" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
@@ -3664,51 +3571,37 @@
         <v>41</v>
       </c>
     </row>
-    <row r="1048545" spans="7:7">
-      <c r="G1048545" s="2"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:B15 A2">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="very good">
+  <conditionalFormatting sqref="A3:B15 A2 G1048541:G1048576">
+    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="very good">
       <formula>NOT(ISERROR(SEARCH("very good",A2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
       <formula>"maybe"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA14 C14:AY15 BD14:DF14 C3:DF4 C6:CL8 C12:CP12 C11:CJ11 CO11:CP11 C13:CJ13 CP13 C10:DF10 C5:CP5 CX8 CO6:CW6 CY6:DF6 CO7:CV8 DA7:DF8 CU11:CV13 DA11:DF11 CU5:DF5 DA12:DC13 DE12 BD15:DC15 C9:DC9">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="very good">
+    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="very good">
       <formula>NOT(ISERROR(SEARCH("very good",C3)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
       <formula>"maybe"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
-      <formula>"no"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1048545:G1048576">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="very good">
-      <formula>NOT(ISERROR(SEARCH("very good",G1048545)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
-      <formula>"maybe"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL13">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="very good">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="very good">
       <formula>NOT(ISERROR(SEARCH("very good",CL13)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"maybe"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>